<commit_message>
fixes datetime columns in metadata to validate xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/deer_mill_catch_metadata.xlsx
+++ b/data-raw/metadata/deer_mill_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-deer-mill-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-deer-mill-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC424700-7094-F446-93E7-D6CA22F7002F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56F168A-BC77-4A45-B1C8-68446A65226B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="520" windowWidth="27040" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="760" windowWidth="27040" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -136,9 +136,6 @@
     <t>lifestage</t>
   </si>
   <si>
-    <t>trap</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>gram</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
 </sst>
 </file>
@@ -453,9 +453,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -545,15 +545,13 @@
       <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="K2" s="2"/>
       <c r="L2" s="10">
         <v>33891</v>
@@ -729,7 +727,7 @@
         <v>17</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>19</v>
@@ -28354,7 +28352,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F24:F991 F1 F3:F22 H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H24:H991 H1 H3:H22 J2" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H24:H991 H1 H3:H22" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28375,13 +28373,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>